<commit_message>
Add message to first add secretary
</commit_message>
<xml_diff>
--- a/public/files/permissions.xlsx
+++ b/public/files/permissions.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spouyt\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="540" yWindow="15" windowWidth="9735" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,13 +31,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,14 +69,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -339,7 +350,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -347,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -364,123 +375,331 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3006</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
+      <c r="A2" s="1">
+        <v>206617</v>
+      </c>
+      <c r="B2" s="2">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3007</v>
-      </c>
-      <c r="B3">
-        <v>11</v>
+      <c r="A3" s="1">
+        <v>217017</v>
+      </c>
+      <c r="B3" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3008</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
+      <c r="A4" s="1">
+        <v>207302</v>
+      </c>
+      <c r="B4" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3009</v>
-      </c>
-      <c r="B5">
-        <v>13</v>
+        <v>211886</v>
+      </c>
+      <c r="B5" s="2">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3010</v>
-      </c>
-      <c r="B6">
-        <v>14</v>
+        <v>201019</v>
+      </c>
+      <c r="B6" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3011</v>
-      </c>
-      <c r="B7">
-        <v>15</v>
+        <v>203703</v>
+      </c>
+      <c r="B7" s="2">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3012</v>
-      </c>
-      <c r="B8">
-        <v>16</v>
+        <v>206022</v>
+      </c>
+      <c r="B8" s="2">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3013</v>
-      </c>
-      <c r="B9">
-        <v>17</v>
+        <v>207096</v>
+      </c>
+      <c r="B9" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3014</v>
-      </c>
-      <c r="B10">
-        <v>18</v>
+        <v>204962</v>
+      </c>
+      <c r="B10" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3015</v>
-      </c>
-      <c r="B11">
-        <v>19</v>
+        <v>206935</v>
+      </c>
+      <c r="B11" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3016</v>
-      </c>
-      <c r="B12">
-        <v>20</v>
+        <v>207774</v>
+      </c>
+      <c r="B12" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3017</v>
-      </c>
-      <c r="B13">
-        <v>21</v>
+        <v>220989</v>
+      </c>
+      <c r="B13" s="2">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3018</v>
-      </c>
-      <c r="B14">
-        <v>22</v>
+        <v>207963</v>
+      </c>
+      <c r="B14" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3019</v>
-      </c>
-      <c r="B15">
-        <v>23</v>
+        <v>202054</v>
+      </c>
+      <c r="B15" s="2">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3020</v>
-      </c>
-      <c r="B16">
-        <v>24</v>
+        <v>206912</v>
+      </c>
+      <c r="B16" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>206931</v>
+      </c>
+      <c r="B17" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>248974</v>
+      </c>
+      <c r="B18" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>209881</v>
+      </c>
+      <c r="B19" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>203594</v>
+      </c>
+      <c r="B20" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>213469</v>
+      </c>
+      <c r="B21" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>204718</v>
+      </c>
+      <c r="B22" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>208000</v>
+      </c>
+      <c r="B23" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>209255</v>
+      </c>
+      <c r="B24" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>207772</v>
+      </c>
+      <c r="B25" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>207624</v>
+      </c>
+      <c r="B26" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>204398</v>
+      </c>
+      <c r="B27" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>212537</v>
+      </c>
+      <c r="B28" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>202933</v>
+      </c>
+      <c r="B29" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>206879</v>
+      </c>
+      <c r="B30" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>209849</v>
+      </c>
+      <c r="B31" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>200187</v>
+      </c>
+      <c r="B32" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>208855</v>
+      </c>
+      <c r="B33" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>206051</v>
+      </c>
+      <c r="B34" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>201991</v>
+      </c>
+      <c r="B35" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>203970</v>
+      </c>
+      <c r="B36" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>302106</v>
+      </c>
+      <c r="B37" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>208761</v>
+      </c>
+      <c r="B38" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>201338</v>
+      </c>
+      <c r="B39" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>303567</v>
+      </c>
+      <c r="B40" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>207728</v>
+      </c>
+      <c r="B41" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>208915</v>
+      </c>
+      <c r="B42" s="2">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>